<commit_message>
took out weights and added hazard examp
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Cox treat only" sheetId="1" r:id="rId1"/>
+    <sheet name="cox everything" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Capeothno</t>
   </si>
@@ -43,6 +43,126 @@
   </si>
   <si>
     <t>The HR</t>
+  </si>
+  <si>
+    <t>hrher22</t>
+  </si>
+  <si>
+    <t>hrher23</t>
+  </si>
+  <si>
+    <t>hrher24</t>
+  </si>
+  <si>
+    <t>I(agebrainmet &gt; 60)TRUE</t>
+  </si>
+  <si>
+    <t>I(timedx &gt; 6)TRUE</t>
+  </si>
+  <si>
+    <t>I(site5)1</t>
+  </si>
+  <si>
+    <t>factor(race2)2</t>
+  </si>
+  <si>
+    <t>factor(race2)3</t>
+  </si>
+  <si>
+    <t>factor(race2)4</t>
+  </si>
+  <si>
+    <t>I(priorn &gt; 2)TRUE</t>
+  </si>
+  <si>
+    <t>braintype2</t>
+  </si>
+  <si>
+    <t>braintype3</t>
+  </si>
+  <si>
+    <t>controlled1</t>
+  </si>
+  <si>
+    <t>relevel(capeothno, ref = "3")1</t>
+  </si>
+  <si>
+    <t>relevel(capeothno, ref = "3")2</t>
+  </si>
+  <si>
+    <t>Pr(&gt;|t|)</t>
+  </si>
+  <si>
+    <t>lo 95</t>
+  </si>
+  <si>
+    <t>hi 95</t>
+  </si>
+  <si>
+    <t>fmi</t>
+  </si>
+  <si>
+    <t>est</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>cox everything table</t>
+  </si>
+  <si>
+    <t>Cox  everything hr and CI</t>
+  </si>
+  <si>
+    <t>(0.529,0.849)</t>
+  </si>
+  <si>
+    <t>(0.551,0.868)</t>
+  </si>
+  <si>
+    <t>(0.321,0.552)</t>
+  </si>
+  <si>
+    <t>(1.154,1.734)</t>
+  </si>
+  <si>
+    <t>(0.533,0.843)</t>
+  </si>
+  <si>
+    <t>(0.634,0.952)</t>
+  </si>
+  <si>
+    <t>(0.714,1.111)</t>
+  </si>
+  <si>
+    <t>(0.952,1.630)</t>
+  </si>
+  <si>
+    <t>(0.385,1.209)</t>
+  </si>
+  <si>
+    <t>(1.108,1.708)</t>
+  </si>
+  <si>
+    <t>(1.280,1.944)</t>
+  </si>
+  <si>
+    <t>(1.061,1.904)</t>
+  </si>
+  <si>
+    <t>(0.514,0.745)</t>
+  </si>
+  <si>
+    <t>(0.536,0.917)</t>
+  </si>
+  <si>
+    <t>(0.416,0.681)</t>
   </si>
 </sst>
 </file>
@@ -50,7 +170,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -81,9 +201,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:H10"/>
     </sheetView>
   </sheetViews>
@@ -475,7 +596,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <f t="shared" ref="C8:I8" si="0">EXP(D3)</f>
+        <f t="shared" ref="D8:F8" si="0">EXP(D3)</f>
         <v>0.65507863311180625</v>
       </c>
       <c r="E8" s="1"/>
@@ -491,7 +612,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <f t="shared" ref="B9:I10" si="1">EXP(B4)</f>
+        <f t="shared" ref="B9:F10" si="1">EXP(B4)</f>
         <v>0.33587036900303813</v>
       </c>
       <c r="C9" s="1"/>
@@ -539,13 +660,698 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>-0.4005512</v>
+      </c>
+      <c r="C3">
+        <v>0.12077876</v>
+      </c>
+      <c r="D3">
+        <v>-3.3164039999999999</v>
+      </c>
+      <c r="E3">
+        <v>3848.7709</v>
+      </c>
+      <c r="F3" s="2">
+        <v>9.2029700000000004E-4</v>
+      </c>
+      <c r="G3">
+        <v>-0.63734767000000003</v>
+      </c>
+      <c r="H3">
+        <v>-0.16375468000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.11304906000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>-0.36866719999999997</v>
+      </c>
+      <c r="C4">
+        <v>0.11556710000000001</v>
+      </c>
+      <c r="D4">
+        <v>-3.1900710000000001</v>
+      </c>
+      <c r="E4">
+        <v>2972.4539</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.437184E-3</v>
+      </c>
+      <c r="G4">
+        <v>-0.59526683000000002</v>
+      </c>
+      <c r="H4">
+        <v>-0.14206758</v>
+      </c>
+      <c r="I4">
+        <v>0.12875969000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>-0.86597670000000004</v>
+      </c>
+      <c r="C5">
+        <v>0.13829511</v>
+      </c>
+      <c r="D5">
+        <v>-6.2618029999999996</v>
+      </c>
+      <c r="E5">
+        <v>5298.1593999999996</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4.105338E-10</v>
+      </c>
+      <c r="G5">
+        <v>-1.1370920900000001</v>
+      </c>
+      <c r="H5">
+        <v>-0.59486136000000001</v>
+      </c>
+      <c r="I5">
+        <v>9.6227999999999994E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0.34676420000000002</v>
+      </c>
+      <c r="C6">
+        <v>0.10395287</v>
+      </c>
+      <c r="D6">
+        <v>3.3357830000000002</v>
+      </c>
+      <c r="E6">
+        <v>4174.1752999999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8.5802640000000004E-4</v>
+      </c>
+      <c r="G6">
+        <v>0.14296128</v>
+      </c>
+      <c r="H6">
+        <v>0.55056720999999997</v>
+      </c>
+      <c r="I6">
+        <v>0.10851916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>-0.39960469999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.11680293</v>
+      </c>
+      <c r="D7">
+        <v>-3.4211870000000002</v>
+      </c>
+      <c r="E7">
+        <v>6520.6544999999996</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6.2731250000000005E-4</v>
+      </c>
+      <c r="G7">
+        <v>-0.62857671000000004</v>
+      </c>
+      <c r="H7">
+        <v>-0.17063262000000001</v>
+      </c>
+      <c r="I7">
+        <v>8.665689E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>-0.25240560000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.10350342999999999</v>
+      </c>
+      <c r="D8">
+        <v>-2.4386199999999998</v>
+      </c>
+      <c r="E8">
+        <v>5262.9686000000002</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.4776289999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>-0.45531522000000002</v>
+      </c>
+      <c r="H8">
+        <v>-4.9495900000000002E-2</v>
+      </c>
+      <c r="I8">
+        <v>9.6551979999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>-0.11602609999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.1127696</v>
+      </c>
+      <c r="D9">
+        <v>-1.028877</v>
+      </c>
+      <c r="E9">
+        <v>9688.5733</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.30356309999999997</v>
+      </c>
+      <c r="G9">
+        <v>-0.33707801999999998</v>
+      </c>
+      <c r="H9">
+        <v>0.10502591</v>
+      </c>
+      <c r="I9">
+        <v>7.0936189999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0.21954270000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.13716639</v>
+      </c>
+      <c r="D10">
+        <v>1.6005579999999999</v>
+      </c>
+      <c r="E10">
+        <v>2751.8678</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.1095897</v>
+      </c>
+      <c r="G10">
+        <v>-4.941678E-2</v>
+      </c>
+      <c r="H10">
+        <v>0.48850218000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.13385673000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>-0.38305400000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.29211806000000001</v>
+      </c>
+      <c r="D11">
+        <v>-1.311299</v>
+      </c>
+      <c r="E11">
+        <v>16936.133699999998</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.18977459999999999</v>
+      </c>
+      <c r="G11">
+        <v>-0.95563582999999996</v>
+      </c>
+      <c r="H11">
+        <v>0.18952774999999999</v>
+      </c>
+      <c r="I11">
+        <v>5.3417149999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>0.31875340000000002</v>
+      </c>
+      <c r="C12">
+        <v>0.11037389</v>
+      </c>
+      <c r="D12">
+        <v>2.8879419999999998</v>
+      </c>
+      <c r="E12">
+        <v>2255.7462</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3.9146529999999997E-3</v>
+      </c>
+      <c r="G12">
+        <v>0.10230842</v>
+      </c>
+      <c r="H12">
+        <v>0.53519837999999997</v>
+      </c>
+      <c r="I12">
+        <v>0.14794494</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>0.45591039999999999</v>
+      </c>
+      <c r="C13">
+        <v>0.10665384999999999</v>
+      </c>
+      <c r="D13">
+        <v>4.2746740000000001</v>
+      </c>
+      <c r="E13">
+        <v>7969.7130999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.9364700000000001E-5</v>
+      </c>
+      <c r="G13">
+        <v>0.24684096999999999</v>
+      </c>
+      <c r="H13">
+        <v>0.66497985999999998</v>
+      </c>
+      <c r="I13">
+        <v>7.8302570000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>0.35135080000000002</v>
+      </c>
+      <c r="C14">
+        <v>0.14914025</v>
+      </c>
+      <c r="D14">
+        <v>2.355842</v>
+      </c>
+      <c r="E14">
+        <v>6279.4548999999997</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.8511360000000001E-2</v>
+      </c>
+      <c r="G14">
+        <v>5.8984960000000003E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.64371668999999998</v>
+      </c>
+      <c r="I14">
+        <v>8.8321540000000004E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>-0.4800796</v>
+      </c>
+      <c r="C15">
+        <v>9.4845390000000002E-2</v>
+      </c>
+      <c r="D15">
+        <v>-5.0617070000000002</v>
+      </c>
+      <c r="E15">
+        <v>1668.1522</v>
+      </c>
+      <c r="F15" s="2">
+        <v>4.6146969999999999E-7</v>
+      </c>
+      <c r="G15">
+        <v>-0.66610813000000002</v>
+      </c>
+      <c r="H15">
+        <v>-0.29405107000000003</v>
+      </c>
+      <c r="I15">
+        <v>0.17220721999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>-0.35491329999999999</v>
+      </c>
+      <c r="C16">
+        <v>0.13687854999999999</v>
+      </c>
+      <c r="D16">
+        <v>-2.5929069999999999</v>
+      </c>
+      <c r="E16">
+        <v>780.05520000000001</v>
+      </c>
+      <c r="F16" s="2">
+        <v>9.6951260000000001E-3</v>
+      </c>
+      <c r="G16">
+        <v>-0.62360727000000005</v>
+      </c>
+      <c r="H16">
+        <v>-8.6219409999999996E-2</v>
+      </c>
+      <c r="I16">
+        <v>0.25241518000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>-0.63092239999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.12600786999999999</v>
+      </c>
+      <c r="D17">
+        <v>-5.0070079999999999</v>
+      </c>
+      <c r="E17">
+        <v>902.14710000000002</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6.648416E-7</v>
+      </c>
+      <c r="G17">
+        <v>-0.87822513000000002</v>
+      </c>
+      <c r="H17">
+        <v>-0.38361977000000003</v>
+      </c>
+      <c r="I17">
+        <v>0.23461335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1">
+        <f>EXP(B3)</f>
+        <v>0.66995066743635856</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" ref="B22:B35" si="0">EXP(B4)</f>
+        <v>0.69165555512085541</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.42064051234007005</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4144831509165601</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67058507592954453</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.776929551527337</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89045198219744226</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2455070299704574</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68177608238349441</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1">
+        <f>EXP(B12)</f>
+        <v>1.3754121064566713</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5776089846686139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1">
+        <f>EXP(B14)</f>
+        <v>1.4209857202793861</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.61873413860845639</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.70123423758149661</v>
+      </c>
+      <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5321007648303484</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -553,7 +1359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
moved stack to the extras
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Cox treat only" sheetId="1" r:id="rId1"/>
-    <sheet name="cox everything" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="cape Cox treat only" sheetId="1" r:id="rId1"/>
+    <sheet name="cape cox everything" sheetId="2" r:id="rId2"/>
+    <sheet name="lapat only treat" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>Capeothno</t>
   </si>
@@ -163,6 +164,66 @@
   </si>
   <si>
     <t>(0.416,0.681)</t>
+  </si>
+  <si>
+    <t>coef</t>
+  </si>
+  <si>
+    <t>exp(coef)</t>
+  </si>
+  <si>
+    <t>(0.304,0.775)</t>
+  </si>
+  <si>
+    <t>(0.313,0.735)</t>
+  </si>
+  <si>
+    <t>lapat vs none</t>
+  </si>
+  <si>
+    <t>Trastuz vs none</t>
+  </si>
+  <si>
+    <t>AC no weight</t>
+  </si>
+  <si>
+    <t>AC weight</t>
+  </si>
+  <si>
+    <t>MI no weight</t>
+  </si>
+  <si>
+    <t>MI weight</t>
+  </si>
+  <si>
+    <t>lower .95</t>
+  </si>
+  <si>
+    <t>upper .95</t>
+  </si>
+  <si>
+    <t>(0.355,0.616)</t>
+  </si>
+  <si>
+    <t>(0.398,0.597)</t>
+  </si>
+  <si>
+    <t>(0.362,0.622)</t>
+  </si>
+  <si>
+    <t>(0.417,0.614)</t>
+  </si>
+  <si>
+    <t>relevel(lapatrasno, ref = "3")1</t>
+  </si>
+  <si>
+    <t>relevel(lapatrasno, ref = "3")2</t>
+  </si>
+  <si>
+    <t>(0.381,0.855)</t>
+  </si>
+  <si>
+    <t>(0.421,0.759)</t>
   </si>
 </sst>
 </file>
@@ -172,13 +233,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,10 +268,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +579,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:H10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -1357,14 +1427,183 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="3" max="6" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.46729999999999999</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.57079999999999997</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.47438010000000003</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.48504550000000002</v>
+      </c>
+      <c r="N3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.48770000000000002</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.56569999999999998</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.50582130000000003</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.4799079</v>
+      </c>
+      <c r="N4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="B2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.57079999999999997</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.56569999999999998</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clarified method and put lapat only table
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>Capeothno</t>
   </si>
@@ -196,12 +196,6 @@
     <t>MI weight</t>
   </si>
   <si>
-    <t>lower .95</t>
-  </si>
-  <si>
-    <t>upper .95</t>
-  </si>
-  <si>
     <t>(0.355,0.616)</t>
   </si>
   <si>
@@ -214,16 +208,40 @@
     <t>(0.417,0.614)</t>
   </si>
   <si>
-    <t>relevel(lapatrasno, ref = "3")1</t>
-  </si>
-  <si>
-    <t>relevel(lapatrasno, ref = "3")2</t>
-  </si>
-  <si>
     <t>(0.381,0.855)</t>
   </si>
   <si>
     <t>(0.421,0.759)</t>
+  </si>
+  <si>
+    <t>HR lo 95</t>
+  </si>
+  <si>
+    <t>HR hi 95</t>
+  </si>
+  <si>
+    <t>relevel(lapatrasno, ref = "2")1</t>
+  </si>
+  <si>
+    <t>relevel(lapatrasno, ref = "2")3</t>
+  </si>
+  <si>
+    <t>(0.763,1.338)</t>
+  </si>
+  <si>
+    <t>(1.361,3.190)</t>
+  </si>
+  <si>
+    <t>Lapat vs Trastuz</t>
+  </si>
+  <si>
+    <t>(0.673,1.28)</t>
+  </si>
+  <si>
+    <t>(0.693,1.324)</t>
+  </si>
+  <si>
+    <t>(0.680,1.496)</t>
   </si>
 </sst>
 </file>
@@ -1427,16 +1445,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="3" max="6" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1475,7 +1494,7 @@
         <v>0.46729999999999999</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>53</v>
@@ -1484,7 +1503,7 @@
         <v>0.57079999999999997</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
@@ -1494,7 +1513,7 @@
         <v>0.47438010000000003</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L3" t="s">
         <v>53</v>
@@ -1514,7 +1533,7 @@
         <v>0.48770000000000002</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -1523,7 +1542,7 @@
         <v>0.56569999999999998</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
@@ -1533,7 +1552,7 @@
         <v>0.50582130000000003</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
         <v>54</v>
@@ -1543,6 +1562,38 @@
       </c>
       <c r="N4" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="J5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.010705</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1553,57 +1604,54 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="B2:D3"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="6" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" t="s">
         <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E1"/>
       <c r="F1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="1">
-        <v>0.57079999999999997</v>
+        <v>1.010705</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="B3" s="1">
-        <v>0.56569999999999998</v>
+        <v>2.0837330000000001</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Took away surv example, added km picture
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cape Cox treat only" sheetId="1" r:id="rId1"/>
     <sheet name="cape cox everything" sheetId="2" r:id="rId2"/>
     <sheet name="lapat only treat" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Lapat everything" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Capeothno</t>
   </si>
@@ -220,18 +221,9 @@
     <t>HR hi 95</t>
   </si>
   <si>
-    <t>relevel(lapatrasno, ref = "2")1</t>
-  </si>
-  <si>
-    <t>relevel(lapatrasno, ref = "2")3</t>
-  </si>
-  <si>
     <t>(0.763,1.338)</t>
   </si>
   <si>
-    <t>(1.361,3.190)</t>
-  </si>
-  <si>
     <t>Lapat vs Trastuz</t>
   </si>
   <si>
@@ -242,6 +234,30 @@
   </si>
   <si>
     <t>(0.680,1.496)</t>
+  </si>
+  <si>
+    <t>relevel((lapatrasno), ref = "3")1</t>
+  </si>
+  <si>
+    <t>relevel((lapatrasno), ref = "3")2</t>
+  </si>
+  <si>
+    <t>(0.257,0.652)</t>
+  </si>
+  <si>
+    <t>(0.249,0.602)</t>
+  </si>
+  <si>
+    <t>AC no weights</t>
+  </si>
+  <si>
+    <t>AC weights</t>
+  </si>
+  <si>
+    <t>MI no weights</t>
+  </si>
+  <si>
+    <t>MI weights</t>
   </si>
 </sst>
 </file>
@@ -251,19 +267,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -286,13 +296,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1566,34 +1573,34 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>0.95799999999999996</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E5">
         <v>1.0089999999999999</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I5">
         <v>0.92700000000000005</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M5" s="1">
         <v>1.010705</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1604,51 +1611,100 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>0.40958319999999998</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>0.38758720000000002</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="D3" sqref="B2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="6" width="9.140625" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
       <c r="B1" t="s">
         <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="E1"/>
       <c r="F1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>67</v>
+      <c r="A2" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="1">
-        <v>1.010705</v>
+        <v>0.40958319999999998</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>68</v>
+      <c r="A3" t="s">
+        <v>73</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0837330000000001</v>
+        <v>0.38758720000000002</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reformatted table and added ps note
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245"/>
   </bookViews>
   <sheets>
     <sheet name="cape Cox treat only" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
   <si>
     <t>Capeothno</t>
   </si>
@@ -236,12 +236,6 @@
     <t>(0.680,1.496)</t>
   </si>
   <si>
-    <t>relevel((lapatrasno), ref = "3")1</t>
-  </si>
-  <si>
-    <t>relevel((lapatrasno), ref = "3")2</t>
-  </si>
-  <si>
     <t>(0.257,0.652)</t>
   </si>
   <si>
@@ -258,6 +252,81 @@
   </si>
   <si>
     <t>MI weights</t>
+  </si>
+  <si>
+    <t>hrher2_proper</t>
+  </si>
+  <si>
+    <t>race22</t>
+  </si>
+  <si>
+    <t>race23</t>
+  </si>
+  <si>
+    <t>race24</t>
+  </si>
+  <si>
+    <t>relevel((lapatrasno), ref = "2")</t>
+  </si>
+  <si>
+    <t>(0.788,1.417)</t>
+  </si>
+  <si>
+    <t>lapat vs trastuz</t>
+  </si>
+  <si>
+    <t>none vs lapa</t>
+  </si>
+  <si>
+    <t>none vs trastuz</t>
+  </si>
+  <si>
+    <t>trastuz vs none</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>(0.328,0.6089)</t>
+  </si>
+  <si>
+    <t>(0.316,0.692)</t>
+  </si>
+  <si>
+    <t>(0.704,1.560)</t>
+  </si>
+  <si>
+    <t>(0.37,0.75)</t>
+  </si>
+  <si>
+    <t>(0.38,0.68)</t>
+  </si>
+  <si>
+    <t>(0.713,1.477)</t>
+  </si>
+  <si>
+    <t>(0.726,1.754)</t>
+  </si>
+  <si>
+    <t>(0.331,0.798)</t>
+  </si>
+  <si>
+    <t>(0.328,0.632)</t>
+  </si>
+  <si>
+    <t>(0.481,0.894)</t>
+  </si>
+  <si>
+    <t>(0.46,0.754)</t>
+  </si>
+  <si>
+    <t>(0.325,0.482)</t>
+  </si>
+  <si>
+    <t>(0.287,0.394)</t>
+  </si>
+  <si>
+    <t>(0.983,1.416)</t>
   </si>
 </sst>
 </file>
@@ -603,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,16 +754,21 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+      <c r="A8" s="1">
         <f>EXP(B3)</f>
         <v>0.39611131846343295</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
         <f t="shared" ref="D8:F8" si="0">EXP(D3)</f>
         <v>0.65507863311180625</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>0.48411364311610855</v>
@@ -706,16 +780,21 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <f t="shared" ref="B9:F10" si="1">EXP(B4)</f>
+      <c r="A9" s="1">
+        <f>EXP(B4)</f>
         <v>0.33587036900303813</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B9:F10" si="1">EXP(D4)</f>
         <v>0.56665762138222464</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
         <v>0.412732828381284</v>
@@ -727,16 +806,21 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <f t="shared" si="1"/>
+      <c r="A10" s="1">
+        <f>EXP(B5)</f>
         <v>1.1793577374485509</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
         <v>1.1560395702680215</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
         <v>1.1729467825827575</v>
@@ -757,7 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -1454,7 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1611,45 +1695,125 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="N5" sqref="A1:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>77</v>
       </c>
-      <c r="H1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K3" s="1">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3">
+        <v>0.52</v>
+      </c>
+      <c r="I3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" s="1">
         <v>0.40958319999999998</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K4" s="1">
+      <c r="M3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="F4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4">
+        <v>0.51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" s="1">
         <v>0.38758720000000002</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5">
+        <v>1.048</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5">
+        <v>1.026</v>
+      </c>
+      <c r="I5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="M5" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1659,52 +1823,209 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="B2:D3"/>
+      <selection activeCell="D13" sqref="B13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>50</v>
       </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
       <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.40958319999999998</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>0.75953139999999997</v>
+      </c>
+      <c r="C2">
+        <v>0.65238430000000003</v>
+      </c>
+      <c r="D2">
+        <v>0.88427619999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.38758720000000002</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>1.4673106</v>
+      </c>
+      <c r="C3">
+        <v>0.98157280000000002</v>
+      </c>
+      <c r="D3">
+        <v>2.1934187999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>0.74280999999999997</v>
+      </c>
+      <c r="C4">
+        <v>0.48186479999999998</v>
+      </c>
+      <c r="D4">
+        <v>1.1450655000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0.76718649999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.53615400000000002</v>
+      </c>
+      <c r="D5">
+        <v>1.0977726000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6">
+        <v>0.70678470000000004</v>
+      </c>
+      <c r="C6">
+        <v>0.49345800000000001</v>
+      </c>
+      <c r="D6">
+        <v>1.0123344999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>1.4149909000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.9155548</v>
+      </c>
+      <c r="D7">
+        <v>2.1868698000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8">
+        <v>0.87172039999999995</v>
+      </c>
+      <c r="C8">
+        <v>0.4668175</v>
+      </c>
+      <c r="D8">
+        <v>1.6278235999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>1.6257097</v>
+      </c>
+      <c r="C9">
+        <v>1.1386544999999999</v>
+      </c>
+      <c r="D9">
+        <v>2.3211010000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>1.2402705999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.8936866</v>
+      </c>
+      <c r="D10">
+        <v>1.7212647999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>1.4636172000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.83515879999999998</v>
+      </c>
+      <c r="D11">
+        <v>2.5649917000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>0.60314599999999996</v>
+      </c>
+      <c r="C12">
+        <v>0.44833450000000002</v>
+      </c>
+      <c r="D12">
+        <v>0.81141439999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.056751</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.78800380000000003</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.4171539</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14">
+        <v>2.5800643999999999</v>
+      </c>
+      <c r="C14">
+        <v>1.6602490999999999</v>
+      </c>
+      <c r="D14">
+        <v>4.0094780999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed one of the cape tables
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>Capeothno</t>
   </si>
@@ -284,9 +284,6 @@
     <t>trastuz vs none</t>
   </si>
   <si>
-    <t>()</t>
-  </si>
-  <si>
     <t>(0.328,0.6089)</t>
   </si>
   <si>
@@ -327,6 +324,27 @@
   </si>
   <si>
     <t>(0.983,1.416)</t>
+  </si>
+  <si>
+    <t>(0.966,1.383)</t>
+  </si>
+  <si>
+    <t>(0.400,0.585)</t>
+  </si>
+  <si>
+    <t>(0.354,0.481</t>
+  </si>
+  <si>
+    <t>(0.981,1.402)</t>
+  </si>
+  <si>
+    <t>(0.543,0.906)</t>
+  </si>
+  <si>
+    <t>(0.470,0.748)</t>
+  </si>
+  <si>
+    <t>X FILL THIS IN</t>
   </si>
 </sst>
 </file>
@@ -673,10 +691,13 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -759,7 +780,7 @@
         <v>0.39611131846343295</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1">
@@ -767,16 +788,21 @@
         <v>0.65507863311180625</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
         <v>0.48411364311610855</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="H8" s="1">
         <f>EXP(I3)</f>
         <v>0.70175579910360797</v>
+      </c>
+      <c r="I8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -785,24 +811,29 @@
         <v>0.33587036900303813</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1">
-        <f t="shared" ref="B9:F10" si="1">EXP(D4)</f>
+        <f t="shared" ref="D9:F10" si="1">EXP(D4)</f>
         <v>0.56665762138222464</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
         <v>0.412732828381284</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="H9" s="1">
         <f>EXP(I4)</f>
         <v>0.59297531984435392</v>
+      </c>
+      <c r="I9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -811,7 +842,7 @@
         <v>1.1793577374485509</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1">
@@ -819,16 +850,21 @@
         <v>1.1560395702680215</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
         <v>1.1729467825827575</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="H10" s="1">
         <f>EXP(I5)</f>
         <v>1.1834485780754032</v>
+      </c>
+      <c r="I10" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1725,19 +1761,19 @@
         <v>0.46800000000000003</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3">
         <v>0.51400000000000001</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3">
         <v>0.52</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K3" t="s">
         <v>85</v>
@@ -1758,19 +1794,19 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4">
         <v>0.45600000000000002</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4">
         <v>0.51</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K4" t="s">
         <v>86</v>
@@ -1791,19 +1827,19 @@
         <v>1.048</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5">
         <v>1.1279999999999999</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5">
         <v>1.026</v>
       </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K5" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Started some of friends edits
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -344,7 +344,7 @@
     <t>(0.470,0.748)</t>
   </si>
   <si>
-    <t>X FILL THIS IN</t>
+    <t>(0.998,1.404)</t>
   </si>
 </sst>
 </file>
@@ -691,7 +691,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Moved more from friend edits, finished mi section
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cape Cox treat only" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
   <si>
     <t>Capeothno</t>
   </si>
@@ -345,6 +345,15 @@
   </si>
   <si>
     <t>(0.998,1.404)</t>
+  </si>
+  <si>
+    <t>Cape. Vs none</t>
+  </si>
+  <si>
+    <t>Other vs. none</t>
+  </si>
+  <si>
+    <t>Cape vs Other</t>
   </si>
 </sst>
 </file>
@@ -690,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,10 +884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1531,7 @@
       <c r="D32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1536,7 +1545,7 @@
       <c r="D33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1550,7 +1559,7 @@
       <c r="D34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1563,6 +1572,47 @@
       </c>
       <c r="D35" s="1"/>
       <c r="F35" s="1"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" t="s">
+        <v>75</v>
+      </c>
+      <c r="J45" t="s">
+        <v>76</v>
+      </c>
+      <c r="M45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>109</v>
+      </c>
+      <c r="M46">
+        <v>0.70123423758149661</v>
+      </c>
+      <c r="N46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="M47">
+        <v>0.5321007648303484</v>
+      </c>
+      <c r="N47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished combining the survival parts
</commit_message>
<xml_diff>
--- a/excel table code.xlsx
+++ b/excel table code.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
   <si>
     <t>Capeothno</t>
   </si>
@@ -354,6 +354,39 @@
   </si>
   <si>
     <t>Cape vs Other</t>
+  </si>
+  <si>
+    <t>(1.100,1.579)</t>
+  </si>
+  <si>
+    <t>(1.109,1.604)</t>
+  </si>
+  <si>
+    <t>(0.443,0.820)</t>
+  </si>
+  <si>
+    <t>(0.340,0.602)</t>
+  </si>
+  <si>
+    <t>(0.530,0.891)</t>
+  </si>
+  <si>
+    <t>(0.416,0.653)</t>
+  </si>
+  <si>
+    <t>(1.078,1.612)</t>
+  </si>
+  <si>
+    <t>(0.595,0.952)</t>
+  </si>
+  <si>
+    <t>(0.474,0.707)</t>
+  </si>
+  <si>
+    <t>1.300</t>
+  </si>
+  <si>
+    <t>(1.076,1.570)</t>
   </si>
 </sst>
 </file>
@@ -392,10 +425,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,8 +1625,26 @@
       <c r="A46" t="s">
         <v>109</v>
       </c>
+      <c r="D46">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="E46" t="s">
+        <v>116</v>
+      </c>
+      <c r="G46">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="H46" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46">
+        <v>0.752</v>
+      </c>
+      <c r="K46" t="s">
+        <v>119</v>
+      </c>
       <c r="M46">
-        <v>0.70123423758149661</v>
+        <v>0.70099999999999996</v>
       </c>
       <c r="N46" t="s">
         <v>47</v>
@@ -1602,8 +1654,26 @@
       <c r="A47" t="s">
         <v>110</v>
       </c>
+      <c r="D47">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="E47" t="s">
+        <v>117</v>
+      </c>
+      <c r="G47">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="H47" t="s">
+        <v>115</v>
+      </c>
+      <c r="J47">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="K47" t="s">
+        <v>120</v>
+      </c>
       <c r="M47">
-        <v>0.5321007648303484</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="N47" t="s">
         <v>48</v>
@@ -1612,6 +1682,30 @@
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>111</v>
+      </c>
+      <c r="D48">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="E48" t="s">
+        <v>118</v>
+      </c>
+      <c r="G48">
+        <v>1.3340000000000001</v>
+      </c>
+      <c r="H48" t="s">
+        <v>113</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K48" t="s">
+        <v>122</v>
+      </c>
+      <c r="M48">
+        <v>1.3169999999999999</v>
+      </c>
+      <c r="N48" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>